<commit_message>
Extent report and add more functions: Edit, Delete, Add multiple test data
</commit_message>
<xml_diff>
--- a/Competition/Competition/TestLibrary/TestData/TestData.xlsx
+++ b/Competition/Competition/TestLibrary/TestData/TestData.xlsx
@@ -1,29 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\mvpstudio-competition\Competition\Competition\TestLibrary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\mvpstudio-competition\Competition\Competition\TestLibrary\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819E5A8A-8407-4CC6-AB03-F5D2D8C29E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD55C8F-E4D3-44E1-90D4-107955E8E678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33975" yWindow="-7665" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-9855" windowWidth="28800" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
     <sheet name="SignIn" sheetId="1" r:id="rId2"/>
     <sheet name="Profile" sheetId="2" r:id="rId3"/>
     <sheet name="ShareSkill" sheetId="4" r:id="rId4"/>
+    <sheet name="NegativeTC" sheetId="6" r:id="rId5"/>
+    <sheet name="ManageListings" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="121">
   <si>
     <t>Url</t>
   </si>
@@ -88,9 +90,6 @@
     <t>Australia</t>
   </si>
   <si>
-    <t>B.Tech</t>
-  </si>
-  <si>
     <t>binhnguyen130320@gmail.com</t>
   </si>
   <si>
@@ -115,9 +114,6 @@
     <t>Industry Connect</t>
   </si>
   <si>
-    <t>Five years experiences as a Game Script Developer</t>
-  </si>
-  <si>
     <t>http://localhost:5000</t>
   </si>
   <si>
@@ -169,15 +165,9 @@
     <t>SpecFlow</t>
   </si>
   <si>
-    <t>Mon,Tue,Wed</t>
-  </si>
-  <si>
     <t>EndTime</t>
   </si>
   <si>
-    <t>BI</t>
-  </si>
-  <si>
     <t>Active</t>
   </si>
   <si>
@@ -197,16 +187,218 @@
   </si>
   <si>
     <t>On-Site</t>
+  </si>
+  <si>
+    <t>isDelete</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>A session about sharing experiences about how to work with ExcelDataReader, AutoIT, XPath Siblings</t>
+  </si>
+  <si>
+    <t>Test Automation</t>
+  </si>
+  <si>
+    <t>AutoIT</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>Hourly basis service</t>
+  </si>
+  <si>
+    <t>Skill-exchange</t>
+  </si>
+  <si>
+    <t>Software Development</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Hidden</t>
+  </si>
+  <si>
+    <t>Agile Methodology and SQL queries</t>
+  </si>
+  <si>
+    <t>I would like to share about agile scrum topics and basic SQL queries.</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t>Page Factory for QA testing</t>
+  </si>
+  <si>
+    <t>If you need help with Page Factory, please get in touch</t>
+  </si>
+  <si>
+    <t>PageFactory</t>
+  </si>
+  <si>
+    <t>On-site</t>
+  </si>
+  <si>
+    <t>ExcelDataReader AutoIT XPath Siblings</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Databases</t>
+  </si>
+  <si>
+    <t>Music &amp; Audio</t>
+  </si>
+  <si>
+    <t>Mixing &amp; Mastering</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Music for fun</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>1100am</t>
+  </si>
+  <si>
+    <t>1100pm</t>
+  </si>
+  <si>
+    <t>0400pm</t>
+  </si>
+  <si>
+    <t>0900pm</t>
+  </si>
+  <si>
+    <t>0900am</t>
+  </si>
+  <si>
+    <t>0700pm</t>
+  </si>
+  <si>
+    <t>0100pm</t>
+  </si>
+  <si>
+    <t>0200pm</t>
+  </si>
+  <si>
+    <t>1130am</t>
+  </si>
+  <si>
+    <t>Sat</t>
+  </si>
+  <si>
+    <t>Animation</t>
+  </si>
+  <si>
+    <t>I will show you how to play the guitar in you free time</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>Test data</t>
+  </si>
+  <si>
+    <t>ErrorMessage</t>
+  </si>
+  <si>
+    <t>SpecFlow Feature Demo ### plus BDD Concept in Csharp</t>
+  </si>
+  <si>
+    <t>Special characters are not allowed.</t>
+  </si>
+  <si>
+    <t>A session discussing about * ?:'"" Automated testing using SpecFlow, BDD, POM.  Requirements: Visual Studio Community version, CSharp programming, basic manual testing knowledge</t>
+  </si>
+  <si>
+    <t>QA, Software Testing</t>
+  </si>
+  <si>
+    <t>AfterClickSaveButton</t>
+  </si>
+  <si>
+    <t>Please complete the form correctly.</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Not test</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>Dataset end</t>
+  </si>
+  <si>
+    <t>Five years experience as a Game Script Developer</t>
+  </si>
+  <si>
+    <t>M.Tech</t>
+  </si>
+  <si>
+    <t>Special characters</t>
+  </si>
+  <si>
+    <t>Duplicate Tags</t>
+  </si>
+  <si>
+    <t>Past date</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>value&gt;10</t>
+  </si>
+  <si>
+    <t>Start Date cannot be set to a day in the past</t>
+  </si>
+  <si>
+    <t>TC_ID</t>
+  </si>
+  <si>
+    <t>TC_007_</t>
+  </si>
+  <si>
+    <t>Start Date shouldn't be greater than End Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,26 +407,50 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,12 +459,28 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -256,25 +488,171 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="26">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="5" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-      <protection locked="0"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="2" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="2" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="5" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="6">
+    <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="4" builtinId="29"/>
+    <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Warning Text" xfId="2" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -613,49 +991,50 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2">
+      <c r="D2" s="6">
         <v>123456</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="6">
         <v>123456</v>
       </c>
     </row>
@@ -672,35 +1051,35 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="1" max="1" width="41.85546875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="30.28515625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="2">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="7">
         <v>123456</v>
       </c>
     </row>
@@ -719,84 +1098,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
-    <col min="10" max="10" width="52.7109375" customWidth="1"/>
+    <col min="1" max="3" width="20.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="52.7109375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" t="s">
-        <v>30</v>
+      <c r="J2" s="6" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -806,133 +1186,988 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7874BCB-1913-41B9-9C3C-AFABE92052E1}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="G2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="15">
+        <v>44814</v>
+      </c>
+      <c r="I2" s="15">
+        <v>44863</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="O2" s="16">
+        <v>10</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="15">
+        <v>44824</v>
+      </c>
+      <c r="I3" s="15">
+        <v>44861</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="J1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" t="s">
-        <v>49</v>
-      </c>
-      <c r="M1" t="s">
-        <v>53</v>
-      </c>
-      <c r="N1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D4" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="15">
+        <v>44831</v>
+      </c>
+      <c r="I4" s="15">
+        <v>44860</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="N4" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="O4" s="16">
+        <v>5</v>
+      </c>
+      <c r="P4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="F2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="15">
+        <v>44824</v>
+      </c>
+      <c r="I5" s="15">
+        <v>44862</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="N5" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="5">
-        <v>44783</v>
-      </c>
-      <c r="I2" s="5">
-        <v>44804</v>
-      </c>
-      <c r="J2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="4">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="L2" s="4">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="M2" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2" t="s">
-        <v>50</v>
-      </c>
-      <c r="O2">
-        <v>10</v>
-      </c>
-      <c r="P2" t="s">
-        <v>51</v>
-      </c>
+      <c r="O5" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95C7CD8-C2D1-4160-A72A-FF070F3655E9}">
+  <dimension ref="A1:Q14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" style="1" customWidth="1"/>
+    <col min="5" max="16" width="14.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="10">
+        <v>44783</v>
+      </c>
+      <c r="I2" s="10">
+        <v>44860</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+    </row>
+    <row r="3" spans="1:17" ht="36" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
+      <c r="B3" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="24"/>
+      <c r="B4" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="13"/>
+    </row>
+    <row r="5" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+    </row>
+    <row r="6" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
+      <c r="B6" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+    </row>
+    <row r="7" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="11"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A2:A4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5F03C3-3F74-4564-83CF-846440B20881}">
+  <dimension ref="A1:R7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="3" width="36.85546875" style="1" customWidth="1"/>
+    <col min="4" max="17" width="11.28515625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="20"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="20"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="20"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="22">
+        <v>44831</v>
+      </c>
+      <c r="J5" s="22">
+        <v>44864</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="L5" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="M5" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="N5" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="O5" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="P5" s="21">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="R5" s="20"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" s="22">
+        <v>44824</v>
+      </c>
+      <c r="J6" s="22">
+        <v>44862</v>
+      </c>
+      <c r="K6" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="L6" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="M6" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="N6" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="O6" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="P6" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q6" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="R6" s="20"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="22">
+        <v>44831</v>
+      </c>
+      <c r="J7" s="22">
+        <v>44864</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="L7" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="M7" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="N7" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="O7" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="P7" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q7" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="R7" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement Negative test case. Modify gitignore
</commit_message>
<xml_diff>
--- a/Competition/Competition/TestLibrary/TestData/TestData.xlsx
+++ b/Competition/Competition/TestLibrary/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\mvpstudio-competition\Competition\Competition\TestLibrary\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD55C8F-E4D3-44E1-90D4-107955E8E678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D620AF-41BD-4305-B7E0-E564EB633249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-9855" windowWidth="28800" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="142">
   <si>
     <t>Url</t>
   </si>
@@ -336,24 +336,9 @@
     <t>A session discussing about * ?:'"" Automated testing using SpecFlow, BDD, POM.  Requirements: Visual Studio Community version, CSharp programming, basic manual testing knowledge</t>
   </si>
   <si>
-    <t>QA, Software Testing</t>
-  </si>
-  <si>
-    <t>AfterClickSaveButton</t>
-  </si>
-  <si>
     <t>Please complete the form correctly.</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>Not test</t>
-  </si>
-  <si>
-    <t>valid</t>
-  </si>
-  <si>
     <t>Dataset end</t>
   </si>
   <si>
@@ -366,28 +351,106 @@
     <t>Special characters</t>
   </si>
   <si>
-    <t>Duplicate Tags</t>
-  </si>
-  <si>
     <t>Past date</t>
   </si>
   <si>
-    <t>Valid</t>
-  </si>
-  <si>
-    <t>value&gt;10</t>
-  </si>
-  <si>
     <t>Start Date cannot be set to a day in the past</t>
   </si>
   <si>
     <t>TC_ID</t>
   </si>
   <si>
-    <t>TC_007_</t>
-  </si>
-  <si>
     <t>Start Date shouldn't be greater than End Date</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>Category is required</t>
+  </si>
+  <si>
+    <t>OutputMessage</t>
+  </si>
+  <si>
+    <t>Actual category message and expected category message do not match.</t>
+  </si>
+  <si>
+    <t>Actual description message and expected description message do not match.</t>
+  </si>
+  <si>
+    <t>Actual title message and expected title message do not match.</t>
+  </si>
+  <si>
+    <t>Actual Subcategory message and expected Subcategory message do not match.</t>
+  </si>
+  <si>
+    <t>Actual Tags message and expected Tags message do not match.</t>
+  </si>
+  <si>
+    <t>Actual StartDate message and expected StartDate message do not match.</t>
+  </si>
+  <si>
+    <t>Actual Skill Exchange Tags message and expected Skill Exchange Tags message do not match.</t>
+  </si>
+  <si>
+    <t>Actual Click Save message and expected Click Save message do not match.</t>
+  </si>
+  <si>
+    <t>No action</t>
+  </si>
+  <si>
+    <t>Title is required</t>
+  </si>
+  <si>
+    <t>Description is required</t>
+  </si>
+  <si>
+    <t>Tags are required</t>
+  </si>
+  <si>
+    <t>Tag is required</t>
+  </si>
+  <si>
+    <t>valid category</t>
+  </si>
+  <si>
+    <t>No subcategory</t>
+  </si>
+  <si>
+    <t>Ignore</t>
+  </si>
+  <si>
+    <t>Ignore no message</t>
+  </si>
+  <si>
+    <t>no input</t>
+  </si>
+  <si>
+    <t>Fill some fields and Click save</t>
+  </si>
+  <si>
+    <t>Subcategory is required</t>
+  </si>
+  <si>
+    <t>isClickSaveFirst</t>
+  </si>
+  <si>
+    <t>Actual result and expected result do not match.</t>
+  </si>
+  <si>
+    <t>value cannot enter</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>no assertion</t>
+  </si>
+  <si>
+    <t>Assert message</t>
   </si>
 </sst>
 </file>
@@ -409,13 +472,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -449,18 +505,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -480,7 +537,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -571,88 +628,118 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="5" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="4" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="2" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="2" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="4" builtinId="29"/>
-    <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
-    <cellStyle name="Input" xfId="1" builtinId="20"/>
+  <cellStyles count="5">
+    <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="3" builtinId="29"/>
+    <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Warning Text" xfId="2" builtinId="11"/>
+    <cellStyle name="Warning Text" xfId="1" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1167,7 +1254,7 @@
         <v>26</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>27</v>
@@ -1176,7 +1263,7 @@
         <v>28</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1189,7 +1276,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,203 +1371,203 @@
       <c r="G2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="15">
+      <c r="H2" s="13">
         <v>44814</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="13">
         <v>44863</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="O2" s="16">
+      <c r="O2" s="14">
         <v>10</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="P2" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="13">
         <v>44824</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="13">
         <v>44861</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="M3" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="N3" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="O3" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="P3" s="14" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="13">
         <v>44831</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="13">
         <v>44860</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="M4" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="N4" s="16" t="s">
+      <c r="N4" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="O4" s="16">
+      <c r="O4" s="14">
         <v>5</v>
       </c>
-      <c r="P4" s="16" t="s">
+      <c r="P4" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="13">
         <v>44824</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="13">
         <v>44862</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="M5" s="16" t="s">
+      <c r="M5" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="N5" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="O5" s="16" t="s">
+      <c r="O5" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="P5" s="16" t="s">
+      <c r="P5" s="14" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
+      <c r="A6" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1490,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D95C7CD8-C2D1-4160-A72A-FF070F3655E9}">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1508,8 +1595,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>118</v>
+      <c r="A1" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>97</v>
@@ -1557,12 +1644,12 @@
         <v>33</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>119</v>
+      <c r="A2" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>98</v>
@@ -1573,215 +1660,344 @@
       <c r="D2" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="E2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="G2" s="9" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="H2" s="10">
         <v>44783</v>
       </c>
-      <c r="I2" s="10">
-        <v>44860</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>88</v>
+      <c r="I2" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="N2" s="9"/>
+        <v>131</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>131</v>
+      </c>
       <c r="O2" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
+        <v>139</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="3" spans="1:17" ht="36" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25" t="s">
+      <c r="E3" s="18"/>
+      <c r="F3" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="84" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="24"/>
-      <c r="B4" s="13" t="s">
+      <c r="E4" s="24"/>
+      <c r="F4" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="O4" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21"/>
+      <c r="B5" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" s="14" t="s">
+      <c r="C5" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="D5" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="E5" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="B6" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="F7" s="18"/>
+      <c r="G7" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="J4" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="M4" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14" t="s">
+      <c r="C8" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="13"/>
-    </row>
-    <row r="5" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-    </row>
-    <row r="6" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25" t="s">
+      <c r="F8" s="24"/>
+      <c r="G8" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-    </row>
-    <row r="7" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="8" t="s">
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="21"/>
+      <c r="B9" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="11"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C9" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="O9" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="P9" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q9" s="12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="48" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="I10" s="18" t="s">
+        <v>111</v>
+      </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -1854,11 +2070,39 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
     </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A2:A4"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1869,7 +2113,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,217 +2199,217 @@
       <c r="O2" s="19"/>
       <c r="P2" s="19"/>
       <c r="Q2" s="19"/>
-      <c r="R2" s="20"/>
+      <c r="R2" s="17"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="20"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="17"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="20"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="17"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="13">
         <v>44831</v>
       </c>
-      <c r="J5" s="22">
+      <c r="J5" s="13">
         <v>44864</v>
       </c>
-      <c r="K5" s="21" t="s">
+      <c r="K5" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="L5" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="M5" s="23" t="s">
+      <c r="M5" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="N5" s="21" t="s">
+      <c r="N5" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="O5" s="21" t="s">
+      <c r="O5" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="P5" s="21">
+      <c r="P5" s="14">
         <v>5</v>
       </c>
-      <c r="Q5" s="21" t="s">
+      <c r="Q5" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="R5" s="20"/>
+      <c r="R5" s="17"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="13">
         <v>44824</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="13">
         <v>44862</v>
       </c>
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="L6" s="23" t="s">
+      <c r="L6" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="M6" s="23" t="s">
+      <c r="M6" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="N6" s="21" t="s">
+      <c r="N6" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="O6" s="21" t="s">
+      <c r="O6" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="P6" s="21" t="s">
+      <c r="P6" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="Q6" s="21" t="s">
+      <c r="Q6" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="R6" s="20"/>
+      <c r="R6" s="17"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="21" t="s">
+      <c r="A7" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="13">
         <v>44831</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="13">
         <v>44864</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="L7" s="23" t="s">
+      <c r="L7" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="M7" s="23" t="s">
+      <c r="M7" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="N7" s="21" t="s">
+      <c r="N7" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="O7" s="21" t="s">
+      <c r="O7" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="P7" s="21" t="s">
+      <c r="P7" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="Q7" s="21" t="s">
+      <c r="Q7" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="R7" s="20"/>
+      <c r="R7" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>